<commit_message>
fix train test flag
</commit_message>
<xml_diff>
--- a/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
+++ b/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A161"/>
+  <dimension ref="A1:A160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1444,117 +1444,110 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>readability</t>
+          <t>word_count</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>word_count</t>
+          <t>num_questions</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>num_questions</t>
+          <t>pos_score</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>pos_score</t>
+          <t>Positiv</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Positiv</t>
+          <t>Negativ</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Negativ</t>
+          <t>Strong</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>Weak</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Weak</t>
+          <t>Active</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>Passive</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Passive</t>
+          <t>Ovrst</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Ovrst</t>
+          <t>Undrst</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Undrst</t>
+          <t>PN</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>SW</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>AP</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>AP</t>
+          <t>OU</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
-        <is>
-          <t>OU</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
         <is>
           <t>TONE1</t>
         </is>

</xml_diff>

<commit_message>
new version of all data with nlp features
</commit_message>
<xml_diff>
--- a/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
+++ b/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A160"/>
+  <dimension ref="A1:A172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,133 +1423,217 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>train_test_80_20</t>
+          <t>Altman_Z_diff</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>num_transparency</t>
+          <t>Ratio_A_diff</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>gf_score</t>
+          <t>Ratio_B_diff</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>word_count</t>
+          <t>Ratio_C_diff</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>num_questions</t>
+          <t>Ratio_D_diff</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>pos_score</t>
+          <t>Ratio_E_diff</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Positiv</t>
+          <t>grossProfitRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Negativ</t>
+          <t>ebitdaratio_diff</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>operatingIncomeRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Weak</t>
+          <t>incomeBeforeTaxRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>netIncomeRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Passive</t>
+          <t>num_transparency</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Ovrst</t>
+          <t>gf_score</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Undrst</t>
+          <t>word_count</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>num_questions</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>pos_score</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>AP</t>
+          <t>Positiv</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>Negativ</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
+          <t>Strong</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Weak</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Passive</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Ovrst</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Undrst</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>PN</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>SW</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>OU</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
           <t>TONE1</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>num_q_by_len</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>pos_score_finbert</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update all data with nlp features
</commit_message>
<xml_diff>
--- a/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
+++ b/Code/Data Loading and Cleaning/All Data/all_data_with_NLP_features_columns_before_drop_of_missing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A172"/>
+  <dimension ref="A1:A205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,252 +1388,483 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>rating_on_previous_fixed_quarter_date</t>
+          <t>currentRatio</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Investment_Grade</t>
+          <t>quickRatio</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Change Direction Since Last Fixed Quarter Date</t>
+          <t>cashRatio</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Change Since Last Fixed Quarter Date</t>
+          <t>returnOnAssets</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>returnOnEquity</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Altman_Z_diff</t>
+          <t>returnOnCapitalEmployed</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Ratio_A_diff</t>
+          <t>EBITtoRevenue</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Ratio_B_diff</t>
+          <t>debtRatio</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Ratio_C_diff</t>
+          <t>debtRatioAlt</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Ratio_D_diff</t>
+          <t>debtEquityRatio</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Ratio_E_diff</t>
+          <t>equityMultiplier</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>grossProfitRatio_diff</t>
+          <t>enterpriseValueMultiplier</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>ebitdaratio_diff</t>
+          <t>operatingCashFlowPerShare</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>operatingIncomeRatio_diff</t>
+          <t>freeCashFlowPerShare</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>incomeBeforeTaxRatio_diff</t>
+          <t>cashPerShare</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>netIncomeRatio_diff</t>
+          <t>operatingCashFlowToSales</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>num_transparency</t>
+          <t>freeCashFlowToOperatingCashFlow</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>gf_score</t>
+          <t>Altman_Z_diff</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>word_count</t>
+          <t>Ratio_A_diff</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>num_questions</t>
+          <t>Ratio_B_diff</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>pos_score</t>
+          <t>Ratio_C_diff</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Positiv</t>
+          <t>Ratio_D_diff</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Negativ</t>
+          <t>Ratio_E_diff</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Strong</t>
+          <t>grossProfitRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Weak</t>
+          <t>ebitdaratio_diff</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Active</t>
+          <t>operatingIncomeRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Passive</t>
+          <t>incomeBeforeTaxRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Ovrst</t>
+          <t>netIncomeRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Undrst</t>
+          <t>rating_on_previous_fixed_quarter_date</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>Investment_Grade</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>SW</t>
+          <t>Change Direction Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>AP</t>
+          <t>Change Since Last Fixed Quarter Date</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>Sector</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>TONE1</t>
+          <t>currentRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>num_q_by_len</t>
+          <t>quickRatio_diff</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
+          <t>cashRatio_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>returnOnAssets_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>returnOnEquity_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>returnOnCapitalEmployed_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>EBITtoRevenue_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>debtRatio_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>debtRatioAlt_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>debtEquityRatio_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>equityMultiplier_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>enterpriseValueMultiplier_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>operatingCashFlowPerShare_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>freeCashFlowPerShare_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>cashPerShare_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>operatingCashFlowToSales_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>freeCashFlowToOperatingCashFlow_diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
           <t>pos_score_finbert</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>num_transparency</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>gf_score</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>word_count</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>num_questions</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Positiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Negativ</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Strong</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Weak</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Passive</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Ovrst</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Undrst</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>PN</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>SW</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>OU</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>tone</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>num_q_by_len</t>
         </is>
       </c>
     </row>

</xml_diff>